<commit_message>
parsing and upload works
</commit_message>
<xml_diff>
--- a/quizsources/testsheet.xlsx
+++ b/quizsources/testsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden.Frobenius\Documents\GitHub\quizbank\quizsources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15CE46E-ABF8-49C8-B89B-672ED9816E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4429E56F-A32C-4D4C-A900-354430063158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97A11575-2E20-4433-8B04-0A070EA7B1C7}"/>
+    <workbookView xWindow="2430" yWindow="1935" windowWidth="21600" windowHeight="11295" xr2:uid="{97A11575-2E20-4433-8B04-0A070EA7B1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Unit</t>
   </si>
@@ -84,6 +84,42 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>be good boy</t>
+  </si>
+  <si>
+    <t>are you a good boy?</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Maybe so</t>
+  </si>
+  <si>
+    <t>are you sure?</t>
+  </si>
+  <si>
+    <t>amazing unit</t>
+  </si>
+  <si>
+    <t>work hard</t>
+  </si>
+  <si>
+    <t>workin' hard or hardly workin'?</t>
+  </si>
+  <si>
+    <t>workin' hard</t>
+  </si>
+  <si>
+    <t>hardly workin'</t>
   </si>
 </sst>
 </file>
@@ -458,20 +494,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7AEFAC-1CA8-456E-8650-442FDCC593DD}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,6 +583,69 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>